<commit_message>
Add the white paper of AI
</commit_message>
<xml_diff>
--- a/MoM_06_02.xlsx
+++ b/MoM_06_02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="博士 JF westbrook" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Items</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>https://www.leiphone.com/news/201611/pGIgY02AfjM1Wjt9.html?viewType=weixin</t>
+  </si>
+  <si>
+    <t>同济的创业的申请每年4月份、10月份各有一次。如果答辩通过了提供资金和场所</t>
   </si>
 </sst>
 </file>
@@ -542,9 +545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
@@ -556,6 +561,11 @@
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>